<commit_message>
COMPLETE as of 7-31-19
</commit_message>
<xml_diff>
--- a/Project2 guidebook.xlsx
+++ b/Project2 guidebook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carol\Documents\GitHub\PROJECT_2_ETL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A22F45CE-AC80-4108-A3EC-654E52C2CFDE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{222B76B0-7079-401A-9613-825139E74331}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" firstSheet="1" activeTab="6" xr2:uid="{9A206AAC-AA4C-4287-BD3A-04550641F7DE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{9A206AAC-AA4C-4287-BD3A-04550641F7DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Roadmap Data" sheetId="3" r:id="rId1"/>
@@ -22,21 +22,23 @@
     <sheet name="Executive Summary" sheetId="9" r:id="rId7"/>
     <sheet name="ERD" sheetId="20" r:id="rId8"/>
     <sheet name="DB SCHEMA" sheetId="18" r:id="rId9"/>
-    <sheet name="aggregated_data view" sheetId="22" r:id="rId10"/>
-    <sheet name="McDlocsAllClean view" sheetId="23" r:id="rId11"/>
+    <sheet name="census data views" sheetId="22" r:id="rId10"/>
+    <sheet name="McDonalds data views" sheetId="23" r:id="rId11"/>
     <sheet name="IRS2016_abridged view" sheetId="25" r:id="rId12"/>
-    <sheet name="Data set locations" sheetId="11" r:id="rId13"/>
-    <sheet name="HEADERS" sheetId="7" r:id="rId14"/>
-    <sheet name="Censusdata Definitions" sheetId="21" r:id="rId15"/>
-    <sheet name="SampleData STARBUCKS" sheetId="8" r:id="rId16"/>
-    <sheet name="SampleData MCDONALDS" sheetId="14" r:id="rId17"/>
-    <sheet name="SampleData CENSUS" sheetId="15" r:id="rId18"/>
-    <sheet name="SampleData WHOLEFOODS" sheetId="16" r:id="rId19"/>
-    <sheet name="SampleData ZipCode" sheetId="17" r:id="rId20"/>
-    <sheet name="PROCESS MAPPING" sheetId="19" r:id="rId21"/>
-    <sheet name="DOCUMENTATION OF USE" sheetId="12" r:id="rId22"/>
-    <sheet name="FINAL REPORT" sheetId="10" r:id="rId23"/>
-    <sheet name="About" sheetId="2" r:id="rId24"/>
+    <sheet name="WFlocs view" sheetId="26" r:id="rId13"/>
+    <sheet name="Zip codes" sheetId="27" r:id="rId14"/>
+    <sheet name="Data set locations" sheetId="11" r:id="rId15"/>
+    <sheet name="HEADERS" sheetId="7" r:id="rId16"/>
+    <sheet name="Censusdata Definitions" sheetId="21" r:id="rId17"/>
+    <sheet name="SampleData STARBUCKS" sheetId="8" r:id="rId18"/>
+    <sheet name="SampleData MCDONALDS" sheetId="14" r:id="rId19"/>
+    <sheet name="SampleData CENSUS" sheetId="15" r:id="rId20"/>
+    <sheet name="SampleData WHOLEFOODS" sheetId="16" r:id="rId21"/>
+    <sheet name="SampleData ZipCode" sheetId="17" r:id="rId22"/>
+    <sheet name="PROCESS MAPPING" sheetId="19" r:id="rId23"/>
+    <sheet name="DOCUMENTATION OF USE" sheetId="12" r:id="rId24"/>
+    <sheet name="FINAL REPORT" sheetId="10" r:id="rId25"/>
+    <sheet name="About" sheetId="2" r:id="rId26"/>
   </sheets>
   <definedNames>
     <definedName name="Activity">RoadmapData[Milestone or Activity]</definedName>
@@ -60,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1251" uniqueCount="709">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1394" uniqueCount="822">
   <si>
     <t>Current</t>
   </si>
@@ -2243,6 +2245,346 @@
   </si>
   <si>
     <t>Our team, John, Nick, Carol and Mohammad used the skills we have learned in the DataAnalytics bootcamp to bring to you a transformed set of data for use in answering potential questions like: Is there any coorelation between Starbucks, McDonalds, WholeFoods and median household income?  or How many Starbucks are located in what zipcodes?   What is the median household income by zipcode?</t>
+  </si>
+  <si>
+    <t>Wf_address</t>
+  </si>
+  <si>
+    <t>Wf_zip</t>
+  </si>
+  <si>
+    <t>327 Russell St Hadley, MA</t>
+  </si>
+  <si>
+    <t>255 Amherst Street Nashua, NH</t>
+  </si>
+  <si>
+    <t>40 Railroad St. Andover, MA</t>
+  </si>
+  <si>
+    <t>170 Great Rd Bedford, MA</t>
+  </si>
+  <si>
+    <t>4004 Bellaire Blvd Houston, TX</t>
+  </si>
+  <si>
+    <t>5269 River Rd Bethesda, MD</t>
+  </si>
+  <si>
+    <t>255 Hartford Ave Bellingham, MA</t>
+  </si>
+  <si>
+    <t>15 Washington Street Brighton, MA</t>
+  </si>
+  <si>
+    <t>115 Prospect St Cambridge, MA</t>
+  </si>
+  <si>
+    <t>4420 Willard Ave. Chevy Chase, MD</t>
+  </si>
+  <si>
+    <t>475 Wilmington
+West Chester Pike Glen Mills, PA</t>
+  </si>
+  <si>
+    <t>753 Cerrillos Rd Santa Fe, NM</t>
+  </si>
+  <si>
+    <t>2955 West Ray Road Chandler, AZ</t>
+  </si>
+  <si>
+    <t>151 Sockanosset Cross Road Cranston, RI</t>
+  </si>
+  <si>
+    <t>150 Ledge Road Darien, CT</t>
+  </si>
+  <si>
+    <t>821 W. Lancaster Ave Wayne, PA</t>
+  </si>
+  <si>
+    <t>300 Legacy Place Dedham, MA</t>
+  </si>
+  <si>
+    <t>3670 W. Dublin-Granville Rd Columbus, OH</t>
+  </si>
+  <si>
+    <t>905 River Road Edgewater, NJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WholeFoods </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                     Wf_address  Wf_zip</t>
+  </si>
+  <si>
+    <t>0       327 Russell St Hadley, MA    1035</t>
+  </si>
+  <si>
+    <t>1   255 Amherst Street Nashua, NH    3063</t>
+  </si>
+  <si>
+    <t>2     40 Railroad St. Andover, MA    1810</t>
+  </si>
+  <si>
+    <t>3        170 Great Rd Bedford, MA    1730</t>
+  </si>
+  <si>
+    <t>4  4004 Bellaire Blvd Houston, TX   77025</t>
+  </si>
+  <si>
+    <t>FILE NAME:  aggregated_data.csv</t>
+  </si>
+  <si>
+    <t>FILE NAME:  McDlocsAllClean.csv</t>
+  </si>
+  <si>
+    <t>File Name:  Wflocs.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  zip      type  decommissioned primary_city state               county  \</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0  501    UNIQUE               0   Holtsville    NY       Suffolk County   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1  544    UNIQUE               0   Holtsville    NY       Suffolk County   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2  601  STANDARD               0     Adjuntas    PR   Adjuntas Municipio   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3  602  STANDARD               0       Aguada    PR     Aguada Municipio   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4  603  STANDARD               0    Aguadilla    PR  Aguadilla Municipio   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">              timezone area_codes world_region country  latitude  longitude  \</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0     America/New_York        631          NaN      US     40.81     -73.04   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1     America/New_York        631          NaN      US     40.81     -73.04   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2  America/Puerto_Rico    787,939          NaN      US     18.16     -66.72   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3  America/Puerto_Rico    787,939          NaN      US     18.38     -67.18   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4  America/Puerto_Rico        787          NaN      US     18.43     -67.15   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   irs_estimated_population_2015  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0                            562  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1                              0  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2                              0  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3                              0  </t>
+  </si>
+  <si>
+    <t>4                              0</t>
+  </si>
+  <si>
+    <t>File name:  zip_codes_cleaned.csv</t>
+  </si>
+  <si>
+    <t>CREATE TABLE Zip_codes (</t>
+  </si>
+  <si>
+    <t>zip VARCHAR(5),</t>
+  </si>
+  <si>
+    <t>type VARCHAR(8),</t>
+  </si>
+  <si>
+    <t>decommissioned INTEGER,</t>
+  </si>
+  <si>
+    <t>primary_city VARCHAR(255),</t>
+  </si>
+  <si>
+    <t>state VARCHAR(2),</t>
+  </si>
+  <si>
+    <t>county VARCHAR(255),</t>
+  </si>
+  <si>
+    <t>timezone VARCHAR(255),</t>
+  </si>
+  <si>
+    <t>area_codes VARCHAR(255),</t>
+  </si>
+  <si>
+    <t>world_region VARCHAR(2),</t>
+  </si>
+  <si>
+    <t>country VARCHAR(2),</t>
+  </si>
+  <si>
+    <t>latitude NUMERIC,</t>
+  </si>
+  <si>
+    <t>longitude NUMERIC,</t>
+  </si>
+  <si>
+    <t>irs_estimated_population_2015 INTEGER,</t>
+  </si>
+  <si>
+    <t>PRIMARY KEY (zip)</t>
+  </si>
+  <si>
+    <t>);</t>
+  </si>
+  <si>
+    <t>CREATE TABLE SbxLocs (</t>
+  </si>
+  <si>
+    <t>Brand VARCHAR(255),</t>
+  </si>
+  <si>
+    <t>Store_Number VARCHAR(255),</t>
+  </si>
+  <si>
+    <t>Store_Name VARCHAR(255),</t>
+  </si>
+  <si>
+    <t>Ownership_Type VARCHAR(255),</t>
+  </si>
+  <si>
+    <t>Street_Address VARCHAR(255),</t>
+  </si>
+  <si>
+    <t>City VARCHAR(255),</t>
+  </si>
+  <si>
+    <t>State_Province VARCHAR(3),</t>
+  </si>
+  <si>
+    <t>Country VARCHAR(2),</t>
+  </si>
+  <si>
+    <t>Postcode VARCHAR(255),</t>
+  </si>
+  <si>
+    <t>Phone_Number VARCHAR(255),</t>
+  </si>
+  <si>
+    <t>Timezone VARCHAR(255),</t>
+  </si>
+  <si>
+    <t>Longitude NUMERIC,</t>
+  </si>
+  <si>
+    <t>Latitude NUMERIC,</t>
+  </si>
+  <si>
+    <t>Postcode2 VARCHAR(5),</t>
+  </si>
+  <si>
+    <t>PRIMARY KEY (Store_Number)</t>
+  </si>
+  <si>
+    <t>CREATE TABLE WFlocs (</t>
+  </si>
+  <si>
+    <t>wf_address VARCHAR(255),</t>
+  </si>
+  <si>
+    <t>wf_zip VARCHAR(5),</t>
+  </si>
+  <si>
+    <t>PRIMARY KEY (wf_address)</t>
+  </si>
+  <si>
+    <t>CREATE TABLE McDLocs (</t>
+  </si>
+  <si>
+    <t>store_number INTEGER,</t>
+  </si>
+  <si>
+    <t>zip_code VARCHAR(5)</t>
+  </si>
+  <si>
+    <t>CREATE TABLE IRS_2016_abridged (</t>
+  </si>
+  <si>
+    <t>zipcode VARCHAR(5),</t>
+  </si>
+  <si>
+    <t>agi_sub INTEGER,</t>
+  </si>
+  <si>
+    <t>N1 INTEGER,</t>
+  </si>
+  <si>
+    <t>NUMDEP INTEGER,</t>
+  </si>
+  <si>
+    <t>N02650 INTEGER,</t>
+  </si>
+  <si>
+    <t>A02650 INTEGER,</t>
+  </si>
+  <si>
+    <t>N00200 INTEGER,</t>
+  </si>
+  <si>
+    <t>A00200 INTEGER,</t>
+  </si>
+  <si>
+    <t>N00900 INTEGER,</t>
+  </si>
+  <si>
+    <t>A00900 INTEGER,</t>
+  </si>
+  <si>
+    <t>N01000 INTEGER,</t>
+  </si>
+  <si>
+    <t>A01000 INTEGER,</t>
+  </si>
+  <si>
+    <t>N02300 INTEGER,</t>
+  </si>
+  <si>
+    <t>A02300 INTEGER,</t>
+  </si>
+  <si>
+    <t>N03210 INTEGER,</t>
+  </si>
+  <si>
+    <t>A03210 INTEGER,</t>
+  </si>
+  <si>
+    <t>PRIMARY KEY (zipcode, state, agi_sub)</t>
+  </si>
+  <si>
+    <t>CREATE TABLE All_comapnies_all_stores (</t>
+  </si>
+  <si>
+    <t>number_sbx INTEGER,</t>
+  </si>
+  <si>
+    <t>number_wf INTEGER,</t>
+  </si>
+  <si>
+    <t>number_mcd INTEGER,</t>
+  </si>
+  <si>
+    <t>PRIMARY KEY (zipcode),</t>
+  </si>
+  <si>
+    <t>FOREIGN KEY (zipcode) REFERENCES Zip_codes(zip)</t>
   </si>
 </sst>
 </file>
@@ -2384,6 +2726,7 @@
       <family val="2"/>
     </font>
     <font>
+      <b/>
       <u/>
       <sz val="11"/>
       <color theme="1"/>
@@ -2517,7 +2860,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -2573,11 +2916,11 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="6">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -2674,11 +3017,17 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -8637,13 +8986,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>294124</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>104571</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -8681,13 +9030,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>104250</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>142680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -8730,13 +9079,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>485558</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>123620</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -8779,13 +9128,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>84600</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>18857</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -8823,13 +9172,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>561910</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>28382</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -8867,6 +9216,148 @@
 </file>
 
 <file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>66357</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>123618</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2721F064-E302-4AA4-8655-B4834D975B1A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="266700" y="1704975"/>
+          <a:ext cx="2542857" cy="1657143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>475171</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>85450</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9483993E-2A0B-4E56-9484-2DFD8769D7B3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="76200" y="4171950"/>
+          <a:ext cx="8628571" cy="2200000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>199801</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>56886</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B235E636-F951-4B0F-AE81-3C8F55FC96A8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8696325" y="4229100"/>
+          <a:ext cx="1790476" cy="2114286"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -9198,7 +9689,7 @@
   </sheetPr>
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
@@ -9393,111 +9884,121 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B3E47C3-30C1-4E3C-9109-3C503B07CF08}">
-  <dimension ref="A1:A20"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20:O20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+    <row r="1" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="36" t="s">
+        <v>737</v>
+      </c>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="52" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="52" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="52" t="s">
         <v>666</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="52" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="52" t="s">
         <v>667</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="52" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="52" t="s">
         <v>668</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="52" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="52" t="s">
         <v>669</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="52" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="52" t="s">
         <v>670</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="52" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="52" t="s">
         <v>671</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="52" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="52" t="s">
         <v>672</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="52" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="52" t="s">
         <v>673</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="52" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="52" t="s">
         <v>674</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="52" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="52" t="s">
         <v>675</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="52" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="52" t="s">
         <v>676</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="52" t="s">
-        <v>677</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" s="52" t="s">
-        <v>678</v>
-      </c>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="6"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="52" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="52" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="52" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="52" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="52" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="52" t="s">
         <v>682</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -9506,45 +10007,58 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F64B88B-E11C-471B-9615-483C3384290A}">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+    <row r="1" spans="1:6" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="54" t="s">
+        <v>738</v>
+      </c>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="52" t="s">
         <v>683</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="52" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="52" t="s">
         <v>684</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="52" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="52" t="s">
         <v>685</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="52" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="52" t="s">
         <v>686</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="52" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="52" t="s">
         <v>687</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="52" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="52" t="s">
         <v>688</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -9552,84 +10066,272 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E350475-E996-4D51-9E14-5CBB803D8273}">
-  <dimension ref="A1:A13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P19" sqref="P19"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+    <row r="1" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="36" t="s">
+        <v>505</v>
+      </c>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="52" t="s">
         <v>699</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="52" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="52" t="s">
         <v>689</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="52" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="52" t="s">
         <v>690</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="52" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="52" t="s">
         <v>691</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="52" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="52" t="s">
         <v>692</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="52" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="52" t="s">
         <v>693</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="52" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="52" t="s">
         <v>694</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="52" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="52" t="s">
         <v>695</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="52" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="52" t="s">
         <v>696</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="52" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="52" t="s">
         <v>697</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="52" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="52" t="s">
         <v>698</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="52" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="52" t="s">
         <v>700</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8BEB458-1293-4349-BC9A-1D08D758F279}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="36" t="s">
+        <v>739</v>
+      </c>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="52" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="52" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="52" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="52" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="52" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="52" t="s">
+        <v>736</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41E80B69-95C6-4AF2-AA54-C7A3E66C6F0A}">
+  <dimension ref="A1:C22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="36" t="s">
+        <v>758</v>
+      </c>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="52" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="52" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="52" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="52" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="52" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="52" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="52" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="52" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="52" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="52" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="52" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="52" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="6"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="52" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="52" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="52" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="52" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="52" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="52" t="s">
+        <v>757</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4961ECBB-ACA3-4D6E-8CED-B5B4E2CFDCEC}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -9672,44 +10374,45 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86F0245D-243B-45D9-B5DC-3B81556DC865}">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="18" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.5" customWidth="1"/>
-    <col min="2" max="2" width="1.75" customWidth="1"/>
-    <col min="3" max="3" width="16.125" customWidth="1"/>
+    <col min="2" max="2" width="1.875" customWidth="1"/>
     <col min="4" max="4" width="1.75" customWidth="1"/>
-    <col min="5" max="5" width="28.5" customWidth="1"/>
-    <col min="6" max="6" width="1.375" customWidth="1"/>
-    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.875" customWidth="1"/>
+    <col min="6" max="6" width="2.625" customWidth="1"/>
+    <col min="8" max="8" width="2.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="57" t="s">
         <v>503</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54" t="s">
+      <c r="B1" s="57"/>
+      <c r="C1" s="57" t="s">
         <v>521</v>
       </c>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54" t="s">
+      <c r="D1" s="57"/>
+      <c r="E1" s="57" t="s">
         <v>620</v>
       </c>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54" t="s">
+      <c r="F1" s="57"/>
+      <c r="G1" s="57" t="s">
         <v>701</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="57"/>
+      <c r="I1" s="57" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
         <v>486</v>
       </c>
@@ -9724,8 +10427,11 @@
       <c r="G2" s="53" t="s">
         <v>702</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I2" s="32" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="32" t="s">
         <v>487</v>
       </c>
@@ -9740,8 +10446,11 @@
       <c r="G3" s="53" t="s">
         <v>703</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I3" s="32" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="32" t="s">
         <v>488</v>
       </c>
@@ -9754,7 +10463,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="32" t="s">
         <v>489</v>
       </c>
@@ -9767,7 +10476,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="32" t="s">
         <v>490</v>
       </c>
@@ -9780,7 +10489,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="32" t="s">
         <v>491</v>
       </c>
@@ -9793,7 +10502,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="32" t="s">
         <v>492</v>
       </c>
@@ -9806,7 +10515,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="32" t="s">
         <v>493</v>
       </c>
@@ -9819,7 +10528,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="32" t="s">
         <v>494</v>
       </c>
@@ -9832,7 +10541,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="32" t="s">
         <v>495</v>
       </c>
@@ -9845,7 +10554,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="32" t="s">
         <v>496</v>
       </c>
@@ -9858,7 +10567,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="32" t="s">
         <v>497</v>
       </c>
@@ -9871,7 +10580,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="32" t="s">
         <v>498</v>
       </c>
@@ -9884,7 +10593,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="32" t="s">
         <v>499</v>
       </c>
@@ -9895,7 +10604,7 @@
       <c r="D15" s="32"/>
       <c r="E15" s="32"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="32" t="s">
         <v>500</v>
       </c>
@@ -9916,10 +10625,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94D0DC97-C559-48D4-9D2C-9F7945055E02}">
   <dimension ref="A1:H151"/>
   <sheetViews>
@@ -12904,7 +13614,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{286E5434-E6D5-4787-846A-5130B644D42B}">
   <dimension ref="A1:O25"/>
   <sheetViews>
@@ -13954,7 +14664,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1124A315-BAD5-485C-A88A-C7198536D8B6}">
   <dimension ref="A1:B25"/>
   <sheetViews>
@@ -14165,1363 +14875,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0E5F682-9AA9-4011-8E1A-4EEDE389EBC8}">
-  <dimension ref="A1:Q25"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:Q25"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
-        <v>486</v>
-      </c>
-      <c r="B1" s="32" t="s">
-        <v>487</v>
-      </c>
-      <c r="C1" s="32" t="s">
-        <v>488</v>
-      </c>
-      <c r="D1" s="32" t="s">
-        <v>489</v>
-      </c>
-      <c r="E1" s="32" t="s">
-        <v>490</v>
-      </c>
-      <c r="F1" s="32" t="s">
-        <v>491</v>
-      </c>
-      <c r="G1" s="32" t="s">
-        <v>492</v>
-      </c>
-      <c r="H1" s="32" t="s">
-        <v>493</v>
-      </c>
-      <c r="I1" s="32" t="s">
-        <v>494</v>
-      </c>
-      <c r="J1" s="32" t="s">
-        <v>495</v>
-      </c>
-      <c r="K1" s="32" t="s">
-        <v>496</v>
-      </c>
-      <c r="L1" s="32" t="s">
-        <v>497</v>
-      </c>
-      <c r="M1" s="32" t="s">
-        <v>498</v>
-      </c>
-      <c r="N1" s="32" t="s">
-        <v>499</v>
-      </c>
-      <c r="O1" s="32" t="s">
-        <v>500</v>
-      </c>
-      <c r="P1" s="32" t="s">
-        <v>501</v>
-      </c>
-      <c r="Q1" s="32" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="32">
-        <v>0</v>
-      </c>
-      <c r="B2" s="32" t="s">
-        <v>504</v>
-      </c>
-      <c r="C2" s="32">
-        <v>1</v>
-      </c>
-      <c r="D2" s="32">
-        <v>815440</v>
-      </c>
-      <c r="E2" s="32">
-        <v>491310</v>
-      </c>
-      <c r="F2" s="32">
-        <v>815440</v>
-      </c>
-      <c r="G2" s="32">
-        <v>10787121</v>
-      </c>
-      <c r="H2" s="32">
-        <v>651680</v>
-      </c>
-      <c r="I2" s="32">
-        <v>8466376</v>
-      </c>
-      <c r="J2" s="32">
-        <v>144430</v>
-      </c>
-      <c r="K2" s="32">
-        <v>765184</v>
-      </c>
-      <c r="L2" s="32">
-        <v>34770</v>
-      </c>
-      <c r="M2" s="32">
-        <v>20594</v>
-      </c>
-      <c r="N2" s="32">
-        <v>22770</v>
-      </c>
-      <c r="O2" s="32">
-        <v>65220</v>
-      </c>
-      <c r="P2" s="32">
-        <v>17110</v>
-      </c>
-      <c r="Q2" s="32">
-        <v>14893</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="32">
-        <v>0</v>
-      </c>
-      <c r="B3" s="32" t="s">
-        <v>504</v>
-      </c>
-      <c r="C3" s="32">
-        <v>2</v>
-      </c>
-      <c r="D3" s="32">
-        <v>495830</v>
-      </c>
-      <c r="E3" s="32">
-        <v>360480</v>
-      </c>
-      <c r="F3" s="32">
-        <v>495830</v>
-      </c>
-      <c r="G3" s="32">
-        <v>18020908</v>
-      </c>
-      <c r="H3" s="32">
-        <v>427840</v>
-      </c>
-      <c r="I3" s="32">
-        <v>14690098</v>
-      </c>
-      <c r="J3" s="32">
-        <v>65350</v>
-      </c>
-      <c r="K3" s="32">
-        <v>258861</v>
-      </c>
-      <c r="L3" s="32">
-        <v>31040</v>
-      </c>
-      <c r="M3" s="32">
-        <v>50118</v>
-      </c>
-      <c r="N3" s="32">
-        <v>15170</v>
-      </c>
-      <c r="O3" s="32">
-        <v>45546</v>
-      </c>
-      <c r="P3" s="32">
-        <v>41490</v>
-      </c>
-      <c r="Q3" s="32">
-        <v>43047</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="32">
-        <v>0</v>
-      </c>
-      <c r="B4" s="32" t="s">
-        <v>504</v>
-      </c>
-      <c r="C4" s="32">
-        <v>3</v>
-      </c>
-      <c r="D4" s="32">
-        <v>263390</v>
-      </c>
-      <c r="E4" s="32">
-        <v>182880</v>
-      </c>
-      <c r="F4" s="32">
-        <v>263390</v>
-      </c>
-      <c r="G4" s="32">
-        <v>16351320</v>
-      </c>
-      <c r="H4" s="32">
-        <v>225610</v>
-      </c>
-      <c r="I4" s="32">
-        <v>12476022</v>
-      </c>
-      <c r="J4" s="32">
-        <v>41390</v>
-      </c>
-      <c r="K4" s="32">
-        <v>259064</v>
-      </c>
-      <c r="L4" s="32">
-        <v>31240</v>
-      </c>
-      <c r="M4" s="32">
-        <v>85650</v>
-      </c>
-      <c r="N4" s="32">
-        <v>7460</v>
-      </c>
-      <c r="O4" s="32">
-        <v>24614</v>
-      </c>
-      <c r="P4" s="32">
-        <v>29110</v>
-      </c>
-      <c r="Q4" s="32">
-        <v>31929</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="32">
-        <v>0</v>
-      </c>
-      <c r="B5" s="32" t="s">
-        <v>504</v>
-      </c>
-      <c r="C5" s="32">
-        <v>4</v>
-      </c>
-      <c r="D5" s="32">
-        <v>167190</v>
-      </c>
-      <c r="E5" s="32">
-        <v>130160</v>
-      </c>
-      <c r="F5" s="32">
-        <v>167190</v>
-      </c>
-      <c r="G5" s="32">
-        <v>14646693</v>
-      </c>
-      <c r="H5" s="32">
-        <v>144290</v>
-      </c>
-      <c r="I5" s="32">
-        <v>10900188</v>
-      </c>
-      <c r="J5" s="32">
-        <v>28910</v>
-      </c>
-      <c r="K5" s="32">
-        <v>240845</v>
-      </c>
-      <c r="L5" s="32">
-        <v>27320</v>
-      </c>
-      <c r="M5" s="32">
-        <v>103892</v>
-      </c>
-      <c r="N5" s="32">
-        <v>3850</v>
-      </c>
-      <c r="O5" s="32">
-        <v>13372</v>
-      </c>
-      <c r="P5" s="32">
-        <v>20610</v>
-      </c>
-      <c r="Q5" s="32">
-        <v>23854</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="32">
-        <v>0</v>
-      </c>
-      <c r="B6" s="32" t="s">
-        <v>504</v>
-      </c>
-      <c r="C6" s="32">
-        <v>5</v>
-      </c>
-      <c r="D6" s="32">
-        <v>217440</v>
-      </c>
-      <c r="E6" s="32">
-        <v>195990</v>
-      </c>
-      <c r="F6" s="32">
-        <v>217440</v>
-      </c>
-      <c r="G6" s="32">
-        <v>29696755</v>
-      </c>
-      <c r="H6" s="32">
-        <v>193550</v>
-      </c>
-      <c r="I6" s="32">
-        <v>21806247</v>
-      </c>
-      <c r="J6" s="32">
-        <v>43180</v>
-      </c>
-      <c r="K6" s="32">
-        <v>684832</v>
-      </c>
-      <c r="L6" s="32">
-        <v>59160</v>
-      </c>
-      <c r="M6" s="32">
-        <v>506542</v>
-      </c>
-      <c r="N6" s="32">
-        <v>2280</v>
-      </c>
-      <c r="O6" s="32">
-        <v>8380</v>
-      </c>
-      <c r="P6" s="32">
-        <v>22870</v>
-      </c>
-      <c r="Q6" s="32">
-        <v>24745</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="32">
-        <v>0</v>
-      </c>
-      <c r="B7" s="32" t="s">
-        <v>504</v>
-      </c>
-      <c r="C7" s="32">
-        <v>6</v>
-      </c>
-      <c r="D7" s="32">
-        <v>57240</v>
-      </c>
-      <c r="E7" s="32">
-        <v>56220</v>
-      </c>
-      <c r="F7" s="32">
-        <v>57230</v>
-      </c>
-      <c r="G7" s="32">
-        <v>26303410</v>
-      </c>
-      <c r="H7" s="32">
-        <v>49810</v>
-      </c>
-      <c r="I7" s="32">
-        <v>12535261</v>
-      </c>
-      <c r="J7" s="32">
-        <v>14800</v>
-      </c>
-      <c r="K7" s="32">
-        <v>925832</v>
-      </c>
-      <c r="L7" s="32">
-        <v>32610</v>
-      </c>
-      <c r="M7" s="32">
-        <v>2195924</v>
-      </c>
-      <c r="N7" s="32">
-        <v>50</v>
-      </c>
-      <c r="O7" s="32">
-        <v>164</v>
-      </c>
-      <c r="P7" s="32">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="32">
-        <v>35004</v>
-      </c>
-      <c r="B8" s="32" t="s">
-        <v>504</v>
-      </c>
-      <c r="C8" s="32">
-        <v>1</v>
-      </c>
-      <c r="D8" s="32">
-        <v>1510</v>
-      </c>
-      <c r="E8" s="32">
-        <v>660</v>
-      </c>
-      <c r="F8" s="32">
-        <v>1510</v>
-      </c>
-      <c r="G8" s="32">
-        <v>19675</v>
-      </c>
-      <c r="H8" s="32">
-        <v>1170</v>
-      </c>
-      <c r="I8" s="32">
-        <v>14653</v>
-      </c>
-      <c r="J8" s="32">
-        <v>260</v>
-      </c>
-      <c r="K8" s="32">
-        <v>1587</v>
-      </c>
-      <c r="L8" s="32">
-        <v>60</v>
-      </c>
-      <c r="M8" s="32">
-        <v>5</v>
-      </c>
-      <c r="N8" s="32">
-        <v>30</v>
-      </c>
-      <c r="O8" s="32">
-        <v>95</v>
-      </c>
-      <c r="P8" s="32">
-        <v>40</v>
-      </c>
-      <c r="Q8" s="32">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="32">
-        <v>35004</v>
-      </c>
-      <c r="B9" s="32" t="s">
-        <v>504</v>
-      </c>
-      <c r="C9" s="32">
-        <v>2</v>
-      </c>
-      <c r="D9" s="32">
-        <v>1410</v>
-      </c>
-      <c r="E9" s="32">
-        <v>900</v>
-      </c>
-      <c r="F9" s="32">
-        <v>1410</v>
-      </c>
-      <c r="G9" s="32">
-        <v>52487</v>
-      </c>
-      <c r="H9" s="32">
-        <v>1240</v>
-      </c>
-      <c r="I9" s="32">
-        <v>43608</v>
-      </c>
-      <c r="J9" s="32">
-        <v>170</v>
-      </c>
-      <c r="K9" s="32">
-        <v>807</v>
-      </c>
-      <c r="L9" s="32">
-        <v>50</v>
-      </c>
-      <c r="M9" s="32">
-        <v>60</v>
-      </c>
-      <c r="N9" s="32">
-        <v>30</v>
-      </c>
-      <c r="O9" s="32">
-        <v>99</v>
-      </c>
-      <c r="P9" s="32">
-        <v>170</v>
-      </c>
-      <c r="Q9" s="32">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="32">
-        <v>35004</v>
-      </c>
-      <c r="B10" s="32" t="s">
-        <v>504</v>
-      </c>
-      <c r="C10" s="32">
-        <v>3</v>
-      </c>
-      <c r="D10" s="32">
-        <v>950</v>
-      </c>
-      <c r="E10" s="32">
-        <v>660</v>
-      </c>
-      <c r="F10" s="32">
-        <v>950</v>
-      </c>
-      <c r="G10" s="32">
-        <v>59519</v>
-      </c>
-      <c r="H10" s="32">
-        <v>870</v>
-      </c>
-      <c r="I10" s="32">
-        <v>49991</v>
-      </c>
-      <c r="J10" s="32">
-        <v>130</v>
-      </c>
-      <c r="K10" s="32">
-        <v>704</v>
-      </c>
-      <c r="L10" s="32">
-        <v>70</v>
-      </c>
-      <c r="M10" s="32">
-        <v>173</v>
-      </c>
-      <c r="N10" s="32">
-        <v>30</v>
-      </c>
-      <c r="O10" s="32">
-        <v>67</v>
-      </c>
-      <c r="P10" s="32">
-        <v>150</v>
-      </c>
-      <c r="Q10" s="32">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="32">
-        <v>35004</v>
-      </c>
-      <c r="B11" s="32" t="s">
-        <v>504</v>
-      </c>
-      <c r="C11" s="32">
-        <v>4</v>
-      </c>
-      <c r="D11" s="32">
-        <v>650</v>
-      </c>
-      <c r="E11" s="32">
-        <v>560</v>
-      </c>
-      <c r="F11" s="32">
-        <v>650</v>
-      </c>
-      <c r="G11" s="32">
-        <v>56657</v>
-      </c>
-      <c r="H11" s="32">
-        <v>610</v>
-      </c>
-      <c r="I11" s="32">
-        <v>48450</v>
-      </c>
-      <c r="J11" s="32">
-        <v>80</v>
-      </c>
-      <c r="K11" s="32">
-        <v>580</v>
-      </c>
-      <c r="L11" s="32">
-        <v>70</v>
-      </c>
-      <c r="M11" s="32">
-        <v>223</v>
-      </c>
-      <c r="N11" s="32">
-        <v>20</v>
-      </c>
-      <c r="O11" s="32">
-        <v>71</v>
-      </c>
-      <c r="P11" s="32">
-        <v>120</v>
-      </c>
-      <c r="Q11" s="32">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="32">
-        <v>35004</v>
-      </c>
-      <c r="B12" s="32" t="s">
-        <v>504</v>
-      </c>
-      <c r="C12" s="32">
-        <v>5</v>
-      </c>
-      <c r="D12" s="32">
-        <v>630</v>
-      </c>
-      <c r="E12" s="32">
-        <v>610</v>
-      </c>
-      <c r="F12" s="32">
-        <v>630</v>
-      </c>
-      <c r="G12" s="32">
-        <v>81672</v>
-      </c>
-      <c r="H12" s="32">
-        <v>600</v>
-      </c>
-      <c r="I12" s="32">
-        <v>67994</v>
-      </c>
-      <c r="J12" s="32">
-        <v>130</v>
-      </c>
-      <c r="K12" s="32">
-        <v>2616</v>
-      </c>
-      <c r="L12" s="32">
-        <v>100</v>
-      </c>
-      <c r="M12" s="32">
-        <v>383</v>
-      </c>
-      <c r="N12" s="32">
-        <v>0</v>
-      </c>
-      <c r="O12" s="32">
-        <v>0</v>
-      </c>
-      <c r="P12" s="32">
-        <v>110</v>
-      </c>
-      <c r="Q12" s="32">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="32">
-        <v>35004</v>
-      </c>
-      <c r="B13" s="32" t="s">
-        <v>504</v>
-      </c>
-      <c r="C13" s="32">
-        <v>6</v>
-      </c>
-      <c r="D13" s="32">
-        <v>60</v>
-      </c>
-      <c r="E13" s="32">
-        <v>40</v>
-      </c>
-      <c r="F13" s="32">
-        <v>60</v>
-      </c>
-      <c r="G13" s="32">
-        <v>20250</v>
-      </c>
-      <c r="H13" s="32">
-        <v>60</v>
-      </c>
-      <c r="I13" s="32">
-        <v>10137</v>
-      </c>
-      <c r="J13" s="32">
-        <v>0</v>
-      </c>
-      <c r="K13" s="32">
-        <v>0</v>
-      </c>
-      <c r="L13" s="32">
-        <v>30</v>
-      </c>
-      <c r="M13" s="32">
-        <v>784</v>
-      </c>
-      <c r="N13" s="32">
-        <v>0</v>
-      </c>
-      <c r="O13" s="32">
-        <v>0</v>
-      </c>
-      <c r="P13" s="32">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="32">
-        <v>35005</v>
-      </c>
-      <c r="B14" s="32" t="s">
-        <v>504</v>
-      </c>
-      <c r="C14" s="32">
-        <v>1</v>
-      </c>
-      <c r="D14" s="32">
-        <v>1310</v>
-      </c>
-      <c r="E14" s="32">
-        <v>830</v>
-      </c>
-      <c r="F14" s="32">
-        <v>1310</v>
-      </c>
-      <c r="G14" s="32">
-        <v>18061</v>
-      </c>
-      <c r="H14" s="32">
-        <v>1050</v>
-      </c>
-      <c r="I14" s="32">
-        <v>14191</v>
-      </c>
-      <c r="J14" s="32">
-        <v>240</v>
-      </c>
-      <c r="K14" s="32">
-        <v>675</v>
-      </c>
-      <c r="L14" s="32">
-        <v>0</v>
-      </c>
-      <c r="M14" s="32">
-        <v>0</v>
-      </c>
-      <c r="N14" s="32">
-        <v>50</v>
-      </c>
-      <c r="O14" s="32">
-        <v>177</v>
-      </c>
-      <c r="P14" s="32">
-        <v>20</v>
-      </c>
-      <c r="Q14" s="32">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="32">
-        <v>35005</v>
-      </c>
-      <c r="B15" s="32" t="s">
-        <v>504</v>
-      </c>
-      <c r="C15" s="32">
-        <v>2</v>
-      </c>
-      <c r="D15" s="32">
-        <v>960</v>
-      </c>
-      <c r="E15" s="32">
-        <v>720</v>
-      </c>
-      <c r="F15" s="32">
-        <v>960</v>
-      </c>
-      <c r="G15" s="32">
-        <v>35066</v>
-      </c>
-      <c r="H15" s="32">
-        <v>840</v>
-      </c>
-      <c r="I15" s="32">
-        <v>29418</v>
-      </c>
-      <c r="J15" s="32">
-        <v>120</v>
-      </c>
-      <c r="K15" s="32">
-        <v>-253</v>
-      </c>
-      <c r="L15" s="32">
-        <v>50</v>
-      </c>
-      <c r="M15" s="32">
-        <v>27</v>
-      </c>
-      <c r="N15" s="32">
-        <v>30</v>
-      </c>
-      <c r="O15" s="32">
-        <v>101</v>
-      </c>
-      <c r="P15" s="32">
-        <v>90</v>
-      </c>
-      <c r="Q15" s="32">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="32">
-        <v>35005</v>
-      </c>
-      <c r="B16" s="32" t="s">
-        <v>504</v>
-      </c>
-      <c r="C16" s="32">
-        <v>3</v>
-      </c>
-      <c r="D16" s="32">
-        <v>450</v>
-      </c>
-      <c r="E16" s="32">
-        <v>340</v>
-      </c>
-      <c r="F16" s="32">
-        <v>450</v>
-      </c>
-      <c r="G16" s="32">
-        <v>27538</v>
-      </c>
-      <c r="H16" s="32">
-        <v>410</v>
-      </c>
-      <c r="I16" s="32">
-        <v>22677</v>
-      </c>
-      <c r="J16" s="32">
-        <v>60</v>
-      </c>
-      <c r="K16" s="32">
-        <v>26</v>
-      </c>
-      <c r="L16" s="32">
-        <v>30</v>
-      </c>
-      <c r="M16" s="32">
-        <v>16</v>
-      </c>
-      <c r="N16" s="32">
-        <v>30</v>
-      </c>
-      <c r="O16" s="32">
-        <v>89</v>
-      </c>
-      <c r="P16" s="32">
-        <v>80</v>
-      </c>
-      <c r="Q16" s="32">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="32">
-        <v>35005</v>
-      </c>
-      <c r="B17" s="32" t="s">
-        <v>504</v>
-      </c>
-      <c r="C17" s="32">
-        <v>4</v>
-      </c>
-      <c r="D17" s="32">
-        <v>200</v>
-      </c>
-      <c r="E17" s="32">
-        <v>140</v>
-      </c>
-      <c r="F17" s="32">
-        <v>200</v>
-      </c>
-      <c r="G17" s="32">
-        <v>17286</v>
-      </c>
-      <c r="H17" s="32">
-        <v>190</v>
-      </c>
-      <c r="I17" s="32">
-        <v>14129</v>
-      </c>
-      <c r="J17" s="32">
-        <v>30</v>
-      </c>
-      <c r="K17" s="32">
-        <v>-85</v>
-      </c>
-      <c r="L17" s="32">
-        <v>40</v>
-      </c>
-      <c r="M17" s="32">
-        <v>24</v>
-      </c>
-      <c r="N17" s="32">
-        <v>0</v>
-      </c>
-      <c r="O17" s="32">
-        <v>0</v>
-      </c>
-      <c r="P17" s="32">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="32">
-        <v>35005</v>
-      </c>
-      <c r="B18" s="32" t="s">
-        <v>504</v>
-      </c>
-      <c r="C18" s="32">
-        <v>5</v>
-      </c>
-      <c r="D18" s="32">
-        <v>180</v>
-      </c>
-      <c r="E18" s="32">
-        <v>140</v>
-      </c>
-      <c r="F18" s="32">
-        <v>180</v>
-      </c>
-      <c r="G18" s="32">
-        <v>23739</v>
-      </c>
-      <c r="H18" s="32">
-        <v>170</v>
-      </c>
-      <c r="I18" s="32">
-        <v>18150</v>
-      </c>
-      <c r="J18" s="32">
-        <v>30</v>
-      </c>
-      <c r="K18" s="32">
-        <v>-95</v>
-      </c>
-      <c r="L18" s="32">
-        <v>0</v>
-      </c>
-      <c r="M18" s="32">
-        <v>0</v>
-      </c>
-      <c r="N18" s="32">
-        <v>0</v>
-      </c>
-      <c r="O18" s="32">
-        <v>0</v>
-      </c>
-      <c r="P18" s="32">
-        <v>20</v>
-      </c>
-      <c r="Q18" s="32">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" s="32">
-        <v>35005</v>
-      </c>
-      <c r="B19" s="32" t="s">
-        <v>504</v>
-      </c>
-      <c r="C19" s="32">
-        <v>6</v>
-      </c>
-      <c r="D19" s="32">
-        <v>0</v>
-      </c>
-      <c r="E19" s="32">
-        <v>0</v>
-      </c>
-      <c r="F19" s="32">
-        <v>0</v>
-      </c>
-      <c r="G19" s="32">
-        <v>0</v>
-      </c>
-      <c r="H19" s="32">
-        <v>0</v>
-      </c>
-      <c r="I19" s="32">
-        <v>0</v>
-      </c>
-      <c r="J19" s="32">
-        <v>0</v>
-      </c>
-      <c r="K19" s="32">
-        <v>0</v>
-      </c>
-      <c r="L19" s="32">
-        <v>0</v>
-      </c>
-      <c r="M19" s="32">
-        <v>0</v>
-      </c>
-      <c r="N19" s="32">
-        <v>0</v>
-      </c>
-      <c r="O19" s="32">
-        <v>0</v>
-      </c>
-      <c r="P19" s="32">
-        <v>0</v>
-      </c>
-      <c r="Q19" s="32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" s="32">
-        <v>35006</v>
-      </c>
-      <c r="B20" s="32" t="s">
-        <v>504</v>
-      </c>
-      <c r="C20" s="32">
-        <v>1</v>
-      </c>
-      <c r="D20" s="32">
-        <v>430</v>
-      </c>
-      <c r="E20" s="32">
-        <v>210</v>
-      </c>
-      <c r="F20" s="32">
-        <v>430</v>
-      </c>
-      <c r="G20" s="32">
-        <v>5786</v>
-      </c>
-      <c r="H20" s="32">
-        <v>340</v>
-      </c>
-      <c r="I20" s="32">
-        <v>4280</v>
-      </c>
-      <c r="J20" s="32">
-        <v>70</v>
-      </c>
-      <c r="K20" s="32">
-        <v>424</v>
-      </c>
-      <c r="L20" s="32">
-        <v>0</v>
-      </c>
-      <c r="M20" s="32">
-        <v>0</v>
-      </c>
-      <c r="N20" s="32">
-        <v>30</v>
-      </c>
-      <c r="O20" s="32">
-        <v>98</v>
-      </c>
-      <c r="P20" s="32">
-        <v>0</v>
-      </c>
-      <c r="Q20" s="32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A21" s="32">
-        <v>35006</v>
-      </c>
-      <c r="B21" s="32" t="s">
-        <v>504</v>
-      </c>
-      <c r="C21" s="32">
-        <v>2</v>
-      </c>
-      <c r="D21" s="32">
-        <v>330</v>
-      </c>
-      <c r="E21" s="32">
-        <v>220</v>
-      </c>
-      <c r="F21" s="32">
-        <v>330</v>
-      </c>
-      <c r="G21" s="32">
-        <v>11957</v>
-      </c>
-      <c r="H21" s="32">
-        <v>280</v>
-      </c>
-      <c r="I21" s="32">
-        <v>8856</v>
-      </c>
-      <c r="J21" s="32">
-        <v>50</v>
-      </c>
-      <c r="K21" s="32">
-        <v>237</v>
-      </c>
-      <c r="L21" s="32">
-        <v>30</v>
-      </c>
-      <c r="M21" s="32">
-        <v>4</v>
-      </c>
-      <c r="N21" s="32">
-        <v>0</v>
-      </c>
-      <c r="O21" s="32">
-        <v>0</v>
-      </c>
-      <c r="P21" s="32">
-        <v>30</v>
-      </c>
-      <c r="Q21" s="32">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A22" s="32">
-        <v>35006</v>
-      </c>
-      <c r="B22" s="32" t="s">
-        <v>504</v>
-      </c>
-      <c r="C22" s="32">
-        <v>3</v>
-      </c>
-      <c r="D22" s="32">
-        <v>190</v>
-      </c>
-      <c r="E22" s="32">
-        <v>150</v>
-      </c>
-      <c r="F22" s="32">
-        <v>190</v>
-      </c>
-      <c r="G22" s="32">
-        <v>11897</v>
-      </c>
-      <c r="H22" s="32">
-        <v>180</v>
-      </c>
-      <c r="I22" s="32">
-        <v>9263</v>
-      </c>
-      <c r="J22" s="32">
-        <v>0</v>
-      </c>
-      <c r="K22" s="32">
-        <v>0</v>
-      </c>
-      <c r="L22" s="32">
-        <v>0</v>
-      </c>
-      <c r="M22" s="32">
-        <v>0</v>
-      </c>
-      <c r="N22" s="32">
-        <v>40</v>
-      </c>
-      <c r="O22" s="32">
-        <v>111</v>
-      </c>
-      <c r="P22" s="32">
-        <v>0</v>
-      </c>
-      <c r="Q22" s="32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A23" s="32">
-        <v>35006</v>
-      </c>
-      <c r="B23" s="32" t="s">
-        <v>504</v>
-      </c>
-      <c r="C23" s="32">
-        <v>4</v>
-      </c>
-      <c r="D23" s="32">
-        <v>120</v>
-      </c>
-      <c r="E23" s="32">
-        <v>120</v>
-      </c>
-      <c r="F23" s="32">
-        <v>120</v>
-      </c>
-      <c r="G23" s="32">
-        <v>10835</v>
-      </c>
-      <c r="H23" s="32">
-        <v>120</v>
-      </c>
-      <c r="I23" s="32">
-        <v>8692</v>
-      </c>
-      <c r="J23" s="32">
-        <v>40</v>
-      </c>
-      <c r="K23" s="32">
-        <v>251</v>
-      </c>
-      <c r="L23" s="32">
-        <v>20</v>
-      </c>
-      <c r="M23" s="32">
-        <v>-8</v>
-      </c>
-      <c r="N23" s="32">
-        <v>0</v>
-      </c>
-      <c r="O23" s="32">
-        <v>0</v>
-      </c>
-      <c r="P23" s="32">
-        <v>20</v>
-      </c>
-      <c r="Q23" s="32">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A24" s="32">
-        <v>35006</v>
-      </c>
-      <c r="B24" s="32" t="s">
-        <v>504</v>
-      </c>
-      <c r="C24" s="32">
-        <v>5</v>
-      </c>
-      <c r="D24" s="32">
-        <v>130</v>
-      </c>
-      <c r="E24" s="32">
-        <v>120</v>
-      </c>
-      <c r="F24" s="32">
-        <v>130</v>
-      </c>
-      <c r="G24" s="32">
-        <v>16943</v>
-      </c>
-      <c r="H24" s="32">
-        <v>120</v>
-      </c>
-      <c r="I24" s="32">
-        <v>12616</v>
-      </c>
-      <c r="J24" s="32">
-        <v>0</v>
-      </c>
-      <c r="K24" s="32">
-        <v>0</v>
-      </c>
-      <c r="L24" s="32">
-        <v>0</v>
-      </c>
-      <c r="M24" s="32">
-        <v>0</v>
-      </c>
-      <c r="N24" s="32">
-        <v>0</v>
-      </c>
-      <c r="O24" s="32">
-        <v>0</v>
-      </c>
-      <c r="P24" s="32">
-        <v>0</v>
-      </c>
-      <c r="Q24" s="32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A25" s="32">
-        <v>35006</v>
-      </c>
-      <c r="B25" s="32" t="s">
-        <v>504</v>
-      </c>
-      <c r="C25" s="32">
-        <v>6</v>
-      </c>
-      <c r="D25" s="32">
-        <v>0</v>
-      </c>
-      <c r="E25" s="32">
-        <v>0</v>
-      </c>
-      <c r="F25" s="32">
-        <v>0</v>
-      </c>
-      <c r="G25" s="32">
-        <v>0</v>
-      </c>
-      <c r="H25" s="32">
-        <v>0</v>
-      </c>
-      <c r="I25" s="32">
-        <v>0</v>
-      </c>
-      <c r="J25" s="32">
-        <v>0</v>
-      </c>
-      <c r="K25" s="32">
-        <v>0</v>
-      </c>
-      <c r="L25" s="32">
-        <v>0</v>
-      </c>
-      <c r="M25" s="32">
-        <v>0</v>
-      </c>
-      <c r="N25" s="32">
-        <v>0</v>
-      </c>
-      <c r="O25" s="32">
-        <v>0</v>
-      </c>
-      <c r="P25" s="32">
-        <v>0</v>
-      </c>
-      <c r="Q25" s="32">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACF980A7-E674-47D2-845F-994311F43960}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView topLeftCell="B3" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="78.75" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -17466,6 +16819,1564 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0E5F682-9AA9-4011-8E1A-4EEDE389EBC8}">
+  <dimension ref="A1:Q25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:Q25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="32" t="s">
+        <v>486</v>
+      </c>
+      <c r="B1" s="32" t="s">
+        <v>487</v>
+      </c>
+      <c r="C1" s="32" t="s">
+        <v>488</v>
+      </c>
+      <c r="D1" s="32" t="s">
+        <v>489</v>
+      </c>
+      <c r="E1" s="32" t="s">
+        <v>490</v>
+      </c>
+      <c r="F1" s="32" t="s">
+        <v>491</v>
+      </c>
+      <c r="G1" s="32" t="s">
+        <v>492</v>
+      </c>
+      <c r="H1" s="32" t="s">
+        <v>493</v>
+      </c>
+      <c r="I1" s="32" t="s">
+        <v>494</v>
+      </c>
+      <c r="J1" s="32" t="s">
+        <v>495</v>
+      </c>
+      <c r="K1" s="32" t="s">
+        <v>496</v>
+      </c>
+      <c r="L1" s="32" t="s">
+        <v>497</v>
+      </c>
+      <c r="M1" s="32" t="s">
+        <v>498</v>
+      </c>
+      <c r="N1" s="32" t="s">
+        <v>499</v>
+      </c>
+      <c r="O1" s="32" t="s">
+        <v>500</v>
+      </c>
+      <c r="P1" s="32" t="s">
+        <v>501</v>
+      </c>
+      <c r="Q1" s="32" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="32">
+        <v>0</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>504</v>
+      </c>
+      <c r="C2" s="32">
+        <v>1</v>
+      </c>
+      <c r="D2" s="32">
+        <v>815440</v>
+      </c>
+      <c r="E2" s="32">
+        <v>491310</v>
+      </c>
+      <c r="F2" s="32">
+        <v>815440</v>
+      </c>
+      <c r="G2" s="32">
+        <v>10787121</v>
+      </c>
+      <c r="H2" s="32">
+        <v>651680</v>
+      </c>
+      <c r="I2" s="32">
+        <v>8466376</v>
+      </c>
+      <c r="J2" s="32">
+        <v>144430</v>
+      </c>
+      <c r="K2" s="32">
+        <v>765184</v>
+      </c>
+      <c r="L2" s="32">
+        <v>34770</v>
+      </c>
+      <c r="M2" s="32">
+        <v>20594</v>
+      </c>
+      <c r="N2" s="32">
+        <v>22770</v>
+      </c>
+      <c r="O2" s="32">
+        <v>65220</v>
+      </c>
+      <c r="P2" s="32">
+        <v>17110</v>
+      </c>
+      <c r="Q2" s="32">
+        <v>14893</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="32">
+        <v>0</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>504</v>
+      </c>
+      <c r="C3" s="32">
+        <v>2</v>
+      </c>
+      <c r="D3" s="32">
+        <v>495830</v>
+      </c>
+      <c r="E3" s="32">
+        <v>360480</v>
+      </c>
+      <c r="F3" s="32">
+        <v>495830</v>
+      </c>
+      <c r="G3" s="32">
+        <v>18020908</v>
+      </c>
+      <c r="H3" s="32">
+        <v>427840</v>
+      </c>
+      <c r="I3" s="32">
+        <v>14690098</v>
+      </c>
+      <c r="J3" s="32">
+        <v>65350</v>
+      </c>
+      <c r="K3" s="32">
+        <v>258861</v>
+      </c>
+      <c r="L3" s="32">
+        <v>31040</v>
+      </c>
+      <c r="M3" s="32">
+        <v>50118</v>
+      </c>
+      <c r="N3" s="32">
+        <v>15170</v>
+      </c>
+      <c r="O3" s="32">
+        <v>45546</v>
+      </c>
+      <c r="P3" s="32">
+        <v>41490</v>
+      </c>
+      <c r="Q3" s="32">
+        <v>43047</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="32">
+        <v>0</v>
+      </c>
+      <c r="B4" s="32" t="s">
+        <v>504</v>
+      </c>
+      <c r="C4" s="32">
+        <v>3</v>
+      </c>
+      <c r="D4" s="32">
+        <v>263390</v>
+      </c>
+      <c r="E4" s="32">
+        <v>182880</v>
+      </c>
+      <c r="F4" s="32">
+        <v>263390</v>
+      </c>
+      <c r="G4" s="32">
+        <v>16351320</v>
+      </c>
+      <c r="H4" s="32">
+        <v>225610</v>
+      </c>
+      <c r="I4" s="32">
+        <v>12476022</v>
+      </c>
+      <c r="J4" s="32">
+        <v>41390</v>
+      </c>
+      <c r="K4" s="32">
+        <v>259064</v>
+      </c>
+      <c r="L4" s="32">
+        <v>31240</v>
+      </c>
+      <c r="M4" s="32">
+        <v>85650</v>
+      </c>
+      <c r="N4" s="32">
+        <v>7460</v>
+      </c>
+      <c r="O4" s="32">
+        <v>24614</v>
+      </c>
+      <c r="P4" s="32">
+        <v>29110</v>
+      </c>
+      <c r="Q4" s="32">
+        <v>31929</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="32">
+        <v>0</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>504</v>
+      </c>
+      <c r="C5" s="32">
+        <v>4</v>
+      </c>
+      <c r="D5" s="32">
+        <v>167190</v>
+      </c>
+      <c r="E5" s="32">
+        <v>130160</v>
+      </c>
+      <c r="F5" s="32">
+        <v>167190</v>
+      </c>
+      <c r="G5" s="32">
+        <v>14646693</v>
+      </c>
+      <c r="H5" s="32">
+        <v>144290</v>
+      </c>
+      <c r="I5" s="32">
+        <v>10900188</v>
+      </c>
+      <c r="J5" s="32">
+        <v>28910</v>
+      </c>
+      <c r="K5" s="32">
+        <v>240845</v>
+      </c>
+      <c r="L5" s="32">
+        <v>27320</v>
+      </c>
+      <c r="M5" s="32">
+        <v>103892</v>
+      </c>
+      <c r="N5" s="32">
+        <v>3850</v>
+      </c>
+      <c r="O5" s="32">
+        <v>13372</v>
+      </c>
+      <c r="P5" s="32">
+        <v>20610</v>
+      </c>
+      <c r="Q5" s="32">
+        <v>23854</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="32">
+        <v>0</v>
+      </c>
+      <c r="B6" s="32" t="s">
+        <v>504</v>
+      </c>
+      <c r="C6" s="32">
+        <v>5</v>
+      </c>
+      <c r="D6" s="32">
+        <v>217440</v>
+      </c>
+      <c r="E6" s="32">
+        <v>195990</v>
+      </c>
+      <c r="F6" s="32">
+        <v>217440</v>
+      </c>
+      <c r="G6" s="32">
+        <v>29696755</v>
+      </c>
+      <c r="H6" s="32">
+        <v>193550</v>
+      </c>
+      <c r="I6" s="32">
+        <v>21806247</v>
+      </c>
+      <c r="J6" s="32">
+        <v>43180</v>
+      </c>
+      <c r="K6" s="32">
+        <v>684832</v>
+      </c>
+      <c r="L6" s="32">
+        <v>59160</v>
+      </c>
+      <c r="M6" s="32">
+        <v>506542</v>
+      </c>
+      <c r="N6" s="32">
+        <v>2280</v>
+      </c>
+      <c r="O6" s="32">
+        <v>8380</v>
+      </c>
+      <c r="P6" s="32">
+        <v>22870</v>
+      </c>
+      <c r="Q6" s="32">
+        <v>24745</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="32">
+        <v>0</v>
+      </c>
+      <c r="B7" s="32" t="s">
+        <v>504</v>
+      </c>
+      <c r="C7" s="32">
+        <v>6</v>
+      </c>
+      <c r="D7" s="32">
+        <v>57240</v>
+      </c>
+      <c r="E7" s="32">
+        <v>56220</v>
+      </c>
+      <c r="F7" s="32">
+        <v>57230</v>
+      </c>
+      <c r="G7" s="32">
+        <v>26303410</v>
+      </c>
+      <c r="H7" s="32">
+        <v>49810</v>
+      </c>
+      <c r="I7" s="32">
+        <v>12535261</v>
+      </c>
+      <c r="J7" s="32">
+        <v>14800</v>
+      </c>
+      <c r="K7" s="32">
+        <v>925832</v>
+      </c>
+      <c r="L7" s="32">
+        <v>32610</v>
+      </c>
+      <c r="M7" s="32">
+        <v>2195924</v>
+      </c>
+      <c r="N7" s="32">
+        <v>50</v>
+      </c>
+      <c r="O7" s="32">
+        <v>164</v>
+      </c>
+      <c r="P7" s="32">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="32">
+        <v>35004</v>
+      </c>
+      <c r="B8" s="32" t="s">
+        <v>504</v>
+      </c>
+      <c r="C8" s="32">
+        <v>1</v>
+      </c>
+      <c r="D8" s="32">
+        <v>1510</v>
+      </c>
+      <c r="E8" s="32">
+        <v>660</v>
+      </c>
+      <c r="F8" s="32">
+        <v>1510</v>
+      </c>
+      <c r="G8" s="32">
+        <v>19675</v>
+      </c>
+      <c r="H8" s="32">
+        <v>1170</v>
+      </c>
+      <c r="I8" s="32">
+        <v>14653</v>
+      </c>
+      <c r="J8" s="32">
+        <v>260</v>
+      </c>
+      <c r="K8" s="32">
+        <v>1587</v>
+      </c>
+      <c r="L8" s="32">
+        <v>60</v>
+      </c>
+      <c r="M8" s="32">
+        <v>5</v>
+      </c>
+      <c r="N8" s="32">
+        <v>30</v>
+      </c>
+      <c r="O8" s="32">
+        <v>95</v>
+      </c>
+      <c r="P8" s="32">
+        <v>40</v>
+      </c>
+      <c r="Q8" s="32">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="32">
+        <v>35004</v>
+      </c>
+      <c r="B9" s="32" t="s">
+        <v>504</v>
+      </c>
+      <c r="C9" s="32">
+        <v>2</v>
+      </c>
+      <c r="D9" s="32">
+        <v>1410</v>
+      </c>
+      <c r="E9" s="32">
+        <v>900</v>
+      </c>
+      <c r="F9" s="32">
+        <v>1410</v>
+      </c>
+      <c r="G9" s="32">
+        <v>52487</v>
+      </c>
+      <c r="H9" s="32">
+        <v>1240</v>
+      </c>
+      <c r="I9" s="32">
+        <v>43608</v>
+      </c>
+      <c r="J9" s="32">
+        <v>170</v>
+      </c>
+      <c r="K9" s="32">
+        <v>807</v>
+      </c>
+      <c r="L9" s="32">
+        <v>50</v>
+      </c>
+      <c r="M9" s="32">
+        <v>60</v>
+      </c>
+      <c r="N9" s="32">
+        <v>30</v>
+      </c>
+      <c r="O9" s="32">
+        <v>99</v>
+      </c>
+      <c r="P9" s="32">
+        <v>170</v>
+      </c>
+      <c r="Q9" s="32">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="32">
+        <v>35004</v>
+      </c>
+      <c r="B10" s="32" t="s">
+        <v>504</v>
+      </c>
+      <c r="C10" s="32">
+        <v>3</v>
+      </c>
+      <c r="D10" s="32">
+        <v>950</v>
+      </c>
+      <c r="E10" s="32">
+        <v>660</v>
+      </c>
+      <c r="F10" s="32">
+        <v>950</v>
+      </c>
+      <c r="G10" s="32">
+        <v>59519</v>
+      </c>
+      <c r="H10" s="32">
+        <v>870</v>
+      </c>
+      <c r="I10" s="32">
+        <v>49991</v>
+      </c>
+      <c r="J10" s="32">
+        <v>130</v>
+      </c>
+      <c r="K10" s="32">
+        <v>704</v>
+      </c>
+      <c r="L10" s="32">
+        <v>70</v>
+      </c>
+      <c r="M10" s="32">
+        <v>173</v>
+      </c>
+      <c r="N10" s="32">
+        <v>30</v>
+      </c>
+      <c r="O10" s="32">
+        <v>67</v>
+      </c>
+      <c r="P10" s="32">
+        <v>150</v>
+      </c>
+      <c r="Q10" s="32">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="32">
+        <v>35004</v>
+      </c>
+      <c r="B11" s="32" t="s">
+        <v>504</v>
+      </c>
+      <c r="C11" s="32">
+        <v>4</v>
+      </c>
+      <c r="D11" s="32">
+        <v>650</v>
+      </c>
+      <c r="E11" s="32">
+        <v>560</v>
+      </c>
+      <c r="F11" s="32">
+        <v>650</v>
+      </c>
+      <c r="G11" s="32">
+        <v>56657</v>
+      </c>
+      <c r="H11" s="32">
+        <v>610</v>
+      </c>
+      <c r="I11" s="32">
+        <v>48450</v>
+      </c>
+      <c r="J11" s="32">
+        <v>80</v>
+      </c>
+      <c r="K11" s="32">
+        <v>580</v>
+      </c>
+      <c r="L11" s="32">
+        <v>70</v>
+      </c>
+      <c r="M11" s="32">
+        <v>223</v>
+      </c>
+      <c r="N11" s="32">
+        <v>20</v>
+      </c>
+      <c r="O11" s="32">
+        <v>71</v>
+      </c>
+      <c r="P11" s="32">
+        <v>120</v>
+      </c>
+      <c r="Q11" s="32">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="32">
+        <v>35004</v>
+      </c>
+      <c r="B12" s="32" t="s">
+        <v>504</v>
+      </c>
+      <c r="C12" s="32">
+        <v>5</v>
+      </c>
+      <c r="D12" s="32">
+        <v>630</v>
+      </c>
+      <c r="E12" s="32">
+        <v>610</v>
+      </c>
+      <c r="F12" s="32">
+        <v>630</v>
+      </c>
+      <c r="G12" s="32">
+        <v>81672</v>
+      </c>
+      <c r="H12" s="32">
+        <v>600</v>
+      </c>
+      <c r="I12" s="32">
+        <v>67994</v>
+      </c>
+      <c r="J12" s="32">
+        <v>130</v>
+      </c>
+      <c r="K12" s="32">
+        <v>2616</v>
+      </c>
+      <c r="L12" s="32">
+        <v>100</v>
+      </c>
+      <c r="M12" s="32">
+        <v>383</v>
+      </c>
+      <c r="N12" s="32">
+        <v>0</v>
+      </c>
+      <c r="O12" s="32">
+        <v>0</v>
+      </c>
+      <c r="P12" s="32">
+        <v>110</v>
+      </c>
+      <c r="Q12" s="32">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="32">
+        <v>35004</v>
+      </c>
+      <c r="B13" s="32" t="s">
+        <v>504</v>
+      </c>
+      <c r="C13" s="32">
+        <v>6</v>
+      </c>
+      <c r="D13" s="32">
+        <v>60</v>
+      </c>
+      <c r="E13" s="32">
+        <v>40</v>
+      </c>
+      <c r="F13" s="32">
+        <v>60</v>
+      </c>
+      <c r="G13" s="32">
+        <v>20250</v>
+      </c>
+      <c r="H13" s="32">
+        <v>60</v>
+      </c>
+      <c r="I13" s="32">
+        <v>10137</v>
+      </c>
+      <c r="J13" s="32">
+        <v>0</v>
+      </c>
+      <c r="K13" s="32">
+        <v>0</v>
+      </c>
+      <c r="L13" s="32">
+        <v>30</v>
+      </c>
+      <c r="M13" s="32">
+        <v>784</v>
+      </c>
+      <c r="N13" s="32">
+        <v>0</v>
+      </c>
+      <c r="O13" s="32">
+        <v>0</v>
+      </c>
+      <c r="P13" s="32">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="32">
+        <v>35005</v>
+      </c>
+      <c r="B14" s="32" t="s">
+        <v>504</v>
+      </c>
+      <c r="C14" s="32">
+        <v>1</v>
+      </c>
+      <c r="D14" s="32">
+        <v>1310</v>
+      </c>
+      <c r="E14" s="32">
+        <v>830</v>
+      </c>
+      <c r="F14" s="32">
+        <v>1310</v>
+      </c>
+      <c r="G14" s="32">
+        <v>18061</v>
+      </c>
+      <c r="H14" s="32">
+        <v>1050</v>
+      </c>
+      <c r="I14" s="32">
+        <v>14191</v>
+      </c>
+      <c r="J14" s="32">
+        <v>240</v>
+      </c>
+      <c r="K14" s="32">
+        <v>675</v>
+      </c>
+      <c r="L14" s="32">
+        <v>0</v>
+      </c>
+      <c r="M14" s="32">
+        <v>0</v>
+      </c>
+      <c r="N14" s="32">
+        <v>50</v>
+      </c>
+      <c r="O14" s="32">
+        <v>177</v>
+      </c>
+      <c r="P14" s="32">
+        <v>20</v>
+      </c>
+      <c r="Q14" s="32">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="32">
+        <v>35005</v>
+      </c>
+      <c r="B15" s="32" t="s">
+        <v>504</v>
+      </c>
+      <c r="C15" s="32">
+        <v>2</v>
+      </c>
+      <c r="D15" s="32">
+        <v>960</v>
+      </c>
+      <c r="E15" s="32">
+        <v>720</v>
+      </c>
+      <c r="F15" s="32">
+        <v>960</v>
+      </c>
+      <c r="G15" s="32">
+        <v>35066</v>
+      </c>
+      <c r="H15" s="32">
+        <v>840</v>
+      </c>
+      <c r="I15" s="32">
+        <v>29418</v>
+      </c>
+      <c r="J15" s="32">
+        <v>120</v>
+      </c>
+      <c r="K15" s="32">
+        <v>-253</v>
+      </c>
+      <c r="L15" s="32">
+        <v>50</v>
+      </c>
+      <c r="M15" s="32">
+        <v>27</v>
+      </c>
+      <c r="N15" s="32">
+        <v>30</v>
+      </c>
+      <c r="O15" s="32">
+        <v>101</v>
+      </c>
+      <c r="P15" s="32">
+        <v>90</v>
+      </c>
+      <c r="Q15" s="32">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="32">
+        <v>35005</v>
+      </c>
+      <c r="B16" s="32" t="s">
+        <v>504</v>
+      </c>
+      <c r="C16" s="32">
+        <v>3</v>
+      </c>
+      <c r="D16" s="32">
+        <v>450</v>
+      </c>
+      <c r="E16" s="32">
+        <v>340</v>
+      </c>
+      <c r="F16" s="32">
+        <v>450</v>
+      </c>
+      <c r="G16" s="32">
+        <v>27538</v>
+      </c>
+      <c r="H16" s="32">
+        <v>410</v>
+      </c>
+      <c r="I16" s="32">
+        <v>22677</v>
+      </c>
+      <c r="J16" s="32">
+        <v>60</v>
+      </c>
+      <c r="K16" s="32">
+        <v>26</v>
+      </c>
+      <c r="L16" s="32">
+        <v>30</v>
+      </c>
+      <c r="M16" s="32">
+        <v>16</v>
+      </c>
+      <c r="N16" s="32">
+        <v>30</v>
+      </c>
+      <c r="O16" s="32">
+        <v>89</v>
+      </c>
+      <c r="P16" s="32">
+        <v>80</v>
+      </c>
+      <c r="Q16" s="32">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" s="32">
+        <v>35005</v>
+      </c>
+      <c r="B17" s="32" t="s">
+        <v>504</v>
+      </c>
+      <c r="C17" s="32">
+        <v>4</v>
+      </c>
+      <c r="D17" s="32">
+        <v>200</v>
+      </c>
+      <c r="E17" s="32">
+        <v>140</v>
+      </c>
+      <c r="F17" s="32">
+        <v>200</v>
+      </c>
+      <c r="G17" s="32">
+        <v>17286</v>
+      </c>
+      <c r="H17" s="32">
+        <v>190</v>
+      </c>
+      <c r="I17" s="32">
+        <v>14129</v>
+      </c>
+      <c r="J17" s="32">
+        <v>30</v>
+      </c>
+      <c r="K17" s="32">
+        <v>-85</v>
+      </c>
+      <c r="L17" s="32">
+        <v>40</v>
+      </c>
+      <c r="M17" s="32">
+        <v>24</v>
+      </c>
+      <c r="N17" s="32">
+        <v>0</v>
+      </c>
+      <c r="O17" s="32">
+        <v>0</v>
+      </c>
+      <c r="P17" s="32">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" s="32">
+        <v>35005</v>
+      </c>
+      <c r="B18" s="32" t="s">
+        <v>504</v>
+      </c>
+      <c r="C18" s="32">
+        <v>5</v>
+      </c>
+      <c r="D18" s="32">
+        <v>180</v>
+      </c>
+      <c r="E18" s="32">
+        <v>140</v>
+      </c>
+      <c r="F18" s="32">
+        <v>180</v>
+      </c>
+      <c r="G18" s="32">
+        <v>23739</v>
+      </c>
+      <c r="H18" s="32">
+        <v>170</v>
+      </c>
+      <c r="I18" s="32">
+        <v>18150</v>
+      </c>
+      <c r="J18" s="32">
+        <v>30</v>
+      </c>
+      <c r="K18" s="32">
+        <v>-95</v>
+      </c>
+      <c r="L18" s="32">
+        <v>0</v>
+      </c>
+      <c r="M18" s="32">
+        <v>0</v>
+      </c>
+      <c r="N18" s="32">
+        <v>0</v>
+      </c>
+      <c r="O18" s="32">
+        <v>0</v>
+      </c>
+      <c r="P18" s="32">
+        <v>20</v>
+      </c>
+      <c r="Q18" s="32">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19" s="32">
+        <v>35005</v>
+      </c>
+      <c r="B19" s="32" t="s">
+        <v>504</v>
+      </c>
+      <c r="C19" s="32">
+        <v>6</v>
+      </c>
+      <c r="D19" s="32">
+        <v>0</v>
+      </c>
+      <c r="E19" s="32">
+        <v>0</v>
+      </c>
+      <c r="F19" s="32">
+        <v>0</v>
+      </c>
+      <c r="G19" s="32">
+        <v>0</v>
+      </c>
+      <c r="H19" s="32">
+        <v>0</v>
+      </c>
+      <c r="I19" s="32">
+        <v>0</v>
+      </c>
+      <c r="J19" s="32">
+        <v>0</v>
+      </c>
+      <c r="K19" s="32">
+        <v>0</v>
+      </c>
+      <c r="L19" s="32">
+        <v>0</v>
+      </c>
+      <c r="M19" s="32">
+        <v>0</v>
+      </c>
+      <c r="N19" s="32">
+        <v>0</v>
+      </c>
+      <c r="O19" s="32">
+        <v>0</v>
+      </c>
+      <c r="P19" s="32">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20" s="32">
+        <v>35006</v>
+      </c>
+      <c r="B20" s="32" t="s">
+        <v>504</v>
+      </c>
+      <c r="C20" s="32">
+        <v>1</v>
+      </c>
+      <c r="D20" s="32">
+        <v>430</v>
+      </c>
+      <c r="E20" s="32">
+        <v>210</v>
+      </c>
+      <c r="F20" s="32">
+        <v>430</v>
+      </c>
+      <c r="G20" s="32">
+        <v>5786</v>
+      </c>
+      <c r="H20" s="32">
+        <v>340</v>
+      </c>
+      <c r="I20" s="32">
+        <v>4280</v>
+      </c>
+      <c r="J20" s="32">
+        <v>70</v>
+      </c>
+      <c r="K20" s="32">
+        <v>424</v>
+      </c>
+      <c r="L20" s="32">
+        <v>0</v>
+      </c>
+      <c r="M20" s="32">
+        <v>0</v>
+      </c>
+      <c r="N20" s="32">
+        <v>30</v>
+      </c>
+      <c r="O20" s="32">
+        <v>98</v>
+      </c>
+      <c r="P20" s="32">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21" s="32">
+        <v>35006</v>
+      </c>
+      <c r="B21" s="32" t="s">
+        <v>504</v>
+      </c>
+      <c r="C21" s="32">
+        <v>2</v>
+      </c>
+      <c r="D21" s="32">
+        <v>330</v>
+      </c>
+      <c r="E21" s="32">
+        <v>220</v>
+      </c>
+      <c r="F21" s="32">
+        <v>330</v>
+      </c>
+      <c r="G21" s="32">
+        <v>11957</v>
+      </c>
+      <c r="H21" s="32">
+        <v>280</v>
+      </c>
+      <c r="I21" s="32">
+        <v>8856</v>
+      </c>
+      <c r="J21" s="32">
+        <v>50</v>
+      </c>
+      <c r="K21" s="32">
+        <v>237</v>
+      </c>
+      <c r="L21" s="32">
+        <v>30</v>
+      </c>
+      <c r="M21" s="32">
+        <v>4</v>
+      </c>
+      <c r="N21" s="32">
+        <v>0</v>
+      </c>
+      <c r="O21" s="32">
+        <v>0</v>
+      </c>
+      <c r="P21" s="32">
+        <v>30</v>
+      </c>
+      <c r="Q21" s="32">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22" s="32">
+        <v>35006</v>
+      </c>
+      <c r="B22" s="32" t="s">
+        <v>504</v>
+      </c>
+      <c r="C22" s="32">
+        <v>3</v>
+      </c>
+      <c r="D22" s="32">
+        <v>190</v>
+      </c>
+      <c r="E22" s="32">
+        <v>150</v>
+      </c>
+      <c r="F22" s="32">
+        <v>190</v>
+      </c>
+      <c r="G22" s="32">
+        <v>11897</v>
+      </c>
+      <c r="H22" s="32">
+        <v>180</v>
+      </c>
+      <c r="I22" s="32">
+        <v>9263</v>
+      </c>
+      <c r="J22" s="32">
+        <v>0</v>
+      </c>
+      <c r="K22" s="32">
+        <v>0</v>
+      </c>
+      <c r="L22" s="32">
+        <v>0</v>
+      </c>
+      <c r="M22" s="32">
+        <v>0</v>
+      </c>
+      <c r="N22" s="32">
+        <v>40</v>
+      </c>
+      <c r="O22" s="32">
+        <v>111</v>
+      </c>
+      <c r="P22" s="32">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23" s="32">
+        <v>35006</v>
+      </c>
+      <c r="B23" s="32" t="s">
+        <v>504</v>
+      </c>
+      <c r="C23" s="32">
+        <v>4</v>
+      </c>
+      <c r="D23" s="32">
+        <v>120</v>
+      </c>
+      <c r="E23" s="32">
+        <v>120</v>
+      </c>
+      <c r="F23" s="32">
+        <v>120</v>
+      </c>
+      <c r="G23" s="32">
+        <v>10835</v>
+      </c>
+      <c r="H23" s="32">
+        <v>120</v>
+      </c>
+      <c r="I23" s="32">
+        <v>8692</v>
+      </c>
+      <c r="J23" s="32">
+        <v>40</v>
+      </c>
+      <c r="K23" s="32">
+        <v>251</v>
+      </c>
+      <c r="L23" s="32">
+        <v>20</v>
+      </c>
+      <c r="M23" s="32">
+        <v>-8</v>
+      </c>
+      <c r="N23" s="32">
+        <v>0</v>
+      </c>
+      <c r="O23" s="32">
+        <v>0</v>
+      </c>
+      <c r="P23" s="32">
+        <v>20</v>
+      </c>
+      <c r="Q23" s="32">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24" s="32">
+        <v>35006</v>
+      </c>
+      <c r="B24" s="32" t="s">
+        <v>504</v>
+      </c>
+      <c r="C24" s="32">
+        <v>5</v>
+      </c>
+      <c r="D24" s="32">
+        <v>130</v>
+      </c>
+      <c r="E24" s="32">
+        <v>120</v>
+      </c>
+      <c r="F24" s="32">
+        <v>130</v>
+      </c>
+      <c r="G24" s="32">
+        <v>16943</v>
+      </c>
+      <c r="H24" s="32">
+        <v>120</v>
+      </c>
+      <c r="I24" s="32">
+        <v>12616</v>
+      </c>
+      <c r="J24" s="32">
+        <v>0</v>
+      </c>
+      <c r="K24" s="32">
+        <v>0</v>
+      </c>
+      <c r="L24" s="32">
+        <v>0</v>
+      </c>
+      <c r="M24" s="32">
+        <v>0</v>
+      </c>
+      <c r="N24" s="32">
+        <v>0</v>
+      </c>
+      <c r="O24" s="32">
+        <v>0</v>
+      </c>
+      <c r="P24" s="32">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25" s="32">
+        <v>35006</v>
+      </c>
+      <c r="B25" s="32" t="s">
+        <v>504</v>
+      </c>
+      <c r="C25" s="32">
+        <v>6</v>
+      </c>
+      <c r="D25" s="32">
+        <v>0</v>
+      </c>
+      <c r="E25" s="32">
+        <v>0</v>
+      </c>
+      <c r="F25" s="32">
+        <v>0</v>
+      </c>
+      <c r="G25" s="32">
+        <v>0</v>
+      </c>
+      <c r="H25" s="32">
+        <v>0</v>
+      </c>
+      <c r="I25" s="32">
+        <v>0</v>
+      </c>
+      <c r="J25" s="32">
+        <v>0</v>
+      </c>
+      <c r="K25" s="32">
+        <v>0</v>
+      </c>
+      <c r="L25" s="32">
+        <v>0</v>
+      </c>
+      <c r="M25" s="32">
+        <v>0</v>
+      </c>
+      <c r="N25" s="32">
+        <v>0</v>
+      </c>
+      <c r="O25" s="32">
+        <v>0</v>
+      </c>
+      <c r="P25" s="32">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="32">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACF980A7-E674-47D2-845F-994311F43960}">
+  <dimension ref="A3:B27"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="6.25" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="32" t="s">
+        <v>709</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="32" t="s">
+        <v>711</v>
+      </c>
+      <c r="B4" s="32">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="32" t="s">
+        <v>712</v>
+      </c>
+      <c r="B5" s="32">
+        <v>3063</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="32" t="s">
+        <v>713</v>
+      </c>
+      <c r="B6" s="32">
+        <v>1810</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="32" t="s">
+        <v>714</v>
+      </c>
+      <c r="B7" s="32">
+        <v>1730</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="32" t="s">
+        <v>715</v>
+      </c>
+      <c r="B8" s="32">
+        <v>77025</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="32" t="s">
+        <v>711</v>
+      </c>
+      <c r="B9" s="32">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="32" t="s">
+        <v>712</v>
+      </c>
+      <c r="B10" s="32">
+        <v>3063</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="32" t="s">
+        <v>713</v>
+      </c>
+      <c r="B11" s="32">
+        <v>1810</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="32" t="s">
+        <v>714</v>
+      </c>
+      <c r="B12" s="32">
+        <v>1730</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="32" t="s">
+        <v>715</v>
+      </c>
+      <c r="B13" s="32">
+        <v>77025</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="32" t="s">
+        <v>716</v>
+      </c>
+      <c r="B14" s="32">
+        <v>20816</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="32" t="s">
+        <v>717</v>
+      </c>
+      <c r="B15" s="32">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="32" t="s">
+        <v>718</v>
+      </c>
+      <c r="B16" s="32">
+        <v>2135</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="32" t="s">
+        <v>719</v>
+      </c>
+      <c r="B17" s="32">
+        <v>2139</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="32" t="s">
+        <v>720</v>
+      </c>
+      <c r="B18" s="32">
+        <v>20815</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A19" s="56" t="s">
+        <v>721</v>
+      </c>
+      <c r="B19" s="32">
+        <v>19342</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="32" t="s">
+        <v>722</v>
+      </c>
+      <c r="B20" s="32">
+        <v>87505</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="32" t="s">
+        <v>723</v>
+      </c>
+      <c r="B21" s="32">
+        <v>85225</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="32" t="s">
+        <v>724</v>
+      </c>
+      <c r="B22" s="32">
+        <v>2920</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="32" t="s">
+        <v>725</v>
+      </c>
+      <c r="B23" s="32">
+        <v>6820</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="32" t="s">
+        <v>726</v>
+      </c>
+      <c r="B24" s="32">
+        <v>19087</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="32" t="s">
+        <v>727</v>
+      </c>
+      <c r="B25" s="32">
+        <v>2026</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="32" t="s">
+        <v>728</v>
+      </c>
+      <c r="B26" s="32">
+        <v>43235</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="32" t="s">
+        <v>729</v>
+      </c>
+      <c r="B27" s="32">
+        <v>7020</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C52BD1F3-8614-47FB-8520-8F84AC9309A6}">
   <dimension ref="A1:N25"/>
   <sheetViews>
@@ -18519,7 +19430,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0609799-2B29-4387-99AD-476DB1B6C820}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -18534,12 +19445,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECDAB935-423E-452F-9936-BE7B79481D49}">
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18567,7 +19478,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59538CFC-128B-4DE1-813A-9CD59F71C524}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -18581,7 +19492,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCAC69EA-C1A4-4627-B44D-E7990BA50FF1}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:A6"/>
@@ -19073,9 +19984,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08C4FB29-866C-48F0-AB09-622953D96A99}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -19084,7 +19993,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>664</v>
       </c>
       <c r="B1" s="55"/>
@@ -19142,7 +20051,7 @@
       <c r="V1" s="36"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="19"/>
+      <c r="A2" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -19156,14 +20065,464 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E85C1529-B540-4536-9E38-79BE90E95F9A}">
-  <dimension ref="A1"/>
+  <dimension ref="A2:B93"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="A71" sqref="A71:C95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="28.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="52" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="52"/>
+      <c r="B3" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="52"/>
+      <c r="B4" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="52"/>
+      <c r="B5" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="52"/>
+      <c r="B6" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="52"/>
+      <c r="B7" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="6"/>
+      <c r="B8" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="52"/>
+      <c r="B9" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="52"/>
+      <c r="B10" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="52"/>
+      <c r="B11" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="52"/>
+      <c r="B12" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="52"/>
+      <c r="B13" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="52"/>
+      <c r="B14" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="6"/>
+      <c r="B15" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="52"/>
+      <c r="B16" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="52" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="52"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="52"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="52" t="s">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="52"/>
+      <c r="B21" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B78" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B79" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B80" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B85" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B87" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B88" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B90" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B91" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B92" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>774</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>